<commit_message>
Updated mapping for Digestive Health
</commit_message>
<xml_diff>
--- a/Excel Documents/ACC Workgroup to Pod Mapping.xlsx
+++ b/Excel Documents/ACC Workgroup to Pod Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git-Repositories\AmbulatoryOptimization\Excel Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmb4f\source\Workspaces\Tom Burgan - My Files\Development\GitRepositories\AmbulatoryOptimization\Excel Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="143">
   <si>
     <t>Workgroup</t>
   </si>
@@ -441,6 +441,18 @@
   </si>
   <si>
     <t>Women's and Children's</t>
+  </si>
+  <si>
+    <t>Update Date</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Unassign from Pod Digestive Health</t>
+  </si>
+  <si>
+    <t>Assign to Pod Digestive Health</t>
   </si>
 </sst>
 </file>
@@ -476,8 +488,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,7 +771,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -767,9 +780,11 @@
     <col min="1" max="1" width="52.85546875" customWidth="1"/>
     <col min="2" max="2" width="82.140625" customWidth="1"/>
     <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -779,13 +794,19 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -793,7 +814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -801,7 +822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -812,7 +833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -823,7 +844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -834,7 +855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -845,7 +866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -856,7 +877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -867,7 +888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -878,7 +899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -889,7 +910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -897,7 +918,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -905,7 +926,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -913,7 +934,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1177,7 +1198,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -1185,7 +1206,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -1193,12 +1214,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -1209,7 +1230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -1220,18 +1241,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>62</v>
       </c>
       <c r="B54" t="s">
         <v>61</v>
       </c>
-      <c r="C54" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="1">
+        <v>43544</v>
+      </c>
+      <c r="E54" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -1239,15 +1263,24 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>65</v>
       </c>
       <c r="B56" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>61</v>
+      </c>
+      <c r="D56" s="1">
+        <v>43544</v>
+      </c>
+      <c r="E56" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -1255,7 +1288,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -1263,7 +1296,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -1271,7 +1304,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -1279,7 +1312,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -1287,7 +1320,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -1295,7 +1328,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -1306,7 +1339,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>76</v>
       </c>

</xml_diff>